<commit_message>
minor typos in generate py
</commit_message>
<xml_diff>
--- a/2 - DLX Compiler/Instruction_Set.xlsx
+++ b/2 - DLX Compiler/Instruction_Set.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\167so\Documents\labs\2 - DLX Compiler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matthew Crump\Documents\reconfigurable-computing\2 - DLX Compiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8162AE1C-D207-4D15-9E40-952C35069E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF52A02-A145-48B4-9C3A-9E497570CEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="210">
   <si>
     <t>Instruction</t>
   </si>
@@ -645,6 +645,12 @@
   </si>
   <si>
     <t>ORI</t>
+  </si>
+  <si>
+    <t>r_comp</t>
+  </si>
+  <si>
+    <t>absolute address</t>
   </si>
 </sst>
 </file>
@@ -901,7 +907,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -973,15 +979,26 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -990,15 +1007,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1672,20 +1683,20 @@
   </sheetPr>
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1705,7 +1716,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
         <v>6</v>
       </c>
@@ -1725,7 +1736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>10</v>
       </c>
@@ -1745,7 +1756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>16</v>
       </c>
@@ -1765,7 +1776,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>21</v>
       </c>
@@ -1785,7 +1796,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>27</v>
       </c>
@@ -1805,7 +1816,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>33</v>
       </c>
@@ -1825,7 +1836,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>36</v>
       </c>
@@ -1845,7 +1856,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>39</v>
       </c>
@@ -1865,7 +1876,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
         <v>43</v>
       </c>
@@ -1885,7 +1896,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>47</v>
       </c>
@@ -1905,7 +1916,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
         <v>50</v>
       </c>
@@ -1925,7 +1936,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>53</v>
       </c>
@@ -1945,7 +1956,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>57</v>
       </c>
@@ -1965,7 +1976,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>61</v>
       </c>
@@ -1985,7 +1996,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="50" t="s">
         <v>207</v>
       </c>
@@ -2005,7 +2016,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>68</v>
       </c>
@@ -2025,7 +2036,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>72</v>
       </c>
@@ -2045,7 +2056,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
         <v>76</v>
       </c>
@@ -2065,7 +2076,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>80</v>
       </c>
@@ -2085,7 +2096,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>84</v>
       </c>
@@ -2105,7 +2116,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>88</v>
       </c>
@@ -2125,7 +2136,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
         <v>92</v>
       </c>
@@ -2145,7 +2156,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
         <v>96</v>
       </c>
@@ -2165,7 +2176,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>100</v>
       </c>
@@ -2185,7 +2196,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>104</v>
       </c>
@@ -2205,7 +2216,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>108</v>
       </c>
@@ -2225,7 +2236,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>111</v>
       </c>
@@ -2245,7 +2256,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>114</v>
       </c>
@@ -2265,7 +2276,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>117</v>
       </c>
@@ -2285,7 +2296,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>120</v>
       </c>
@@ -2305,7 +2316,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>123</v>
       </c>
@@ -2325,7 +2336,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>126</v>
       </c>
@@ -2345,7 +2356,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>130</v>
       </c>
@@ -2365,7 +2376,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
         <v>134</v>
       </c>
@@ -2385,7 +2396,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>137</v>
       </c>
@@ -2405,7 +2416,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
         <v>140</v>
       </c>
@@ -2425,7 +2436,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>144</v>
       </c>
@@ -2445,7 +2456,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
         <v>148</v>
       </c>
@@ -2465,7 +2476,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>151</v>
       </c>
@@ -2485,7 +2496,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
         <v>154</v>
       </c>
@@ -2505,7 +2516,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>158</v>
       </c>
@@ -2525,7 +2536,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
         <v>162</v>
       </c>
@@ -2545,7 +2556,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
         <v>166</v>
       </c>
@@ -2565,7 +2576,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>170</v>
       </c>
@@ -2585,7 +2596,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>176</v>
       </c>
@@ -2605,7 +2616,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
         <v>180</v>
       </c>
@@ -2625,7 +2636,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>185</v>
       </c>
@@ -2645,7 +2656,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
         <v>190</v>
       </c>
@@ -2665,7 +2676,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>194</v>
       </c>
@@ -2705,16 +2716,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6:AG6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="33" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2815,11 +2828,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="51" t="s">
         <v>198</v>
       </c>
       <c r="C2" s="52"/>
@@ -2827,28 +2840,28 @@
       <c r="E2" s="52"/>
       <c r="F2" s="52"/>
       <c r="G2" s="53"/>
-      <c r="H2" s="58" t="s">
+      <c r="H2" s="54" t="s">
         <v>199</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="51" t="s">
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57" t="s">
         <v>186</v>
       </c>
       <c r="N2" s="52"/>
       <c r="O2" s="52"/>
       <c r="P2" s="52"/>
       <c r="Q2" s="53"/>
-      <c r="R2" s="61" t="s">
+      <c r="R2" s="58" t="s">
         <v>200</v>
       </c>
       <c r="S2" s="52"/>
       <c r="T2" s="52"/>
       <c r="U2" s="52"/>
       <c r="V2" s="53"/>
-      <c r="W2" s="62" t="s">
+      <c r="W2" s="59" t="s">
         <v>201</v>
       </c>
       <c r="X2" s="52"/>
@@ -2862,11 +2875,11 @@
       <c r="AF2" s="52"/>
       <c r="AG2" s="53"/>
     </row>
-    <row r="3" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="51" t="s">
         <v>198</v>
       </c>
       <c r="C3" s="52"/>
@@ -2874,21 +2887,21 @@
       <c r="E3" s="52"/>
       <c r="F3" s="52"/>
       <c r="G3" s="53"/>
-      <c r="H3" s="57" t="s">
+      <c r="H3" s="62" t="s">
         <v>199</v>
       </c>
       <c r="I3" s="52"/>
       <c r="J3" s="52"/>
       <c r="K3" s="52"/>
       <c r="L3" s="53"/>
-      <c r="M3" s="51" t="s">
+      <c r="M3" s="57" t="s">
         <v>186</v>
       </c>
       <c r="N3" s="52"/>
       <c r="O3" s="52"/>
       <c r="P3" s="52"/>
       <c r="Q3" s="53"/>
-      <c r="R3" s="54" t="s">
+      <c r="R3" s="60" t="s">
         <v>202</v>
       </c>
       <c r="S3" s="52"/>
@@ -2907,11 +2920,11 @@
       <c r="AF3" s="52"/>
       <c r="AG3" s="53"/>
     </row>
-    <row r="4" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="51" t="s">
         <v>198</v>
       </c>
       <c r="C4" s="52"/>
@@ -2919,7 +2932,7 @@
       <c r="E4" s="52"/>
       <c r="F4" s="52"/>
       <c r="G4" s="53"/>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="61" t="s">
         <v>203</v>
       </c>
       <c r="I4" s="52"/>
@@ -2948,11 +2961,11 @@
       <c r="AF4" s="52"/>
       <c r="AG4" s="53"/>
     </row>
-    <row r="5" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="51" t="s">
         <v>198</v>
       </c>
       <c r="C5" s="52"/>
@@ -2960,21 +2973,21 @@
       <c r="E5" s="52"/>
       <c r="F5" s="52"/>
       <c r="G5" s="53"/>
-      <c r="H5" s="57" t="s">
+      <c r="H5" s="62" t="s">
         <v>204</v>
       </c>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="52"/>
       <c r="L5" s="53"/>
-      <c r="M5" s="51" t="s">
+      <c r="M5" s="57" t="s">
         <v>205</v>
       </c>
       <c r="N5" s="52"/>
       <c r="O5" s="52"/>
       <c r="P5" s="52"/>
       <c r="Q5" s="53"/>
-      <c r="R5" s="54" t="s">
+      <c r="R5" s="60" t="s">
         <v>206</v>
       </c>
       <c r="S5" s="52"/>
@@ -2993,13 +3006,54 @@
       <c r="AF5" s="52"/>
       <c r="AG5" s="53"/>
     </row>
+    <row r="6" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="62" t="s">
+        <v>208</v>
+      </c>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="65" t="s">
+        <v>209</v>
+      </c>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="63"/>
+      <c r="W6" s="63"/>
+      <c r="X6" s="63"/>
+      <c r="Y6" s="63"/>
+      <c r="Z6" s="63"/>
+      <c r="AA6" s="63"/>
+      <c r="AB6" s="63"/>
+      <c r="AC6" s="63"/>
+      <c r="AD6" s="63"/>
+      <c r="AE6" s="63"/>
+      <c r="AF6" s="63"/>
+      <c r="AG6" s="64"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="W2:AG2"/>
+  <mergeCells count="18">
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="M6:AG6"/>
     <mergeCell ref="M3:Q3"/>
     <mergeCell ref="R3:AG3"/>
     <mergeCell ref="B4:G4"/>
@@ -3010,7 +3064,13 @@
     <mergeCell ref="R5:AG5"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="H3:L3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="W2:AG2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Execute stage initial draft
</commit_message>
<xml_diff>
--- a/2 - DLX Compiler/Instruction_Set.xlsx
+++ b/2 - DLX Compiler/Instruction_Set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matthew Crump\Documents\reconfigurable-computing\2 - DLX Compiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF52A02-A145-48B4-9C3A-9E497570CEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF87D21-4CE7-4F45-A2EA-49A556AFEBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="211">
   <si>
     <t>Instruction</t>
   </si>
@@ -651,13 +651,16 @@
   </si>
   <si>
     <t>absolute address</t>
+  </si>
+  <si>
+    <t>R31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -680,6 +683,11 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -984,32 +992,32 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1683,8 +1691,8 @@
   </sheetPr>
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2719,7 +2727,7 @@
   <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:AG6"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2840,28 +2848,28 @@
       <c r="E2" s="52"/>
       <c r="F2" s="52"/>
       <c r="G2" s="53"/>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="60" t="s">
         <v>199</v>
       </c>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="57" t="s">
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="58" t="s">
         <v>186</v>
       </c>
       <c r="N2" s="52"/>
       <c r="O2" s="52"/>
       <c r="P2" s="52"/>
       <c r="Q2" s="53"/>
-      <c r="R2" s="58" t="s">
+      <c r="R2" s="63" t="s">
         <v>200</v>
       </c>
       <c r="S2" s="52"/>
       <c r="T2" s="52"/>
       <c r="U2" s="52"/>
       <c r="V2" s="53"/>
-      <c r="W2" s="59" t="s">
+      <c r="W2" s="64" t="s">
         <v>201</v>
       </c>
       <c r="X2" s="52"/>
@@ -2887,21 +2895,21 @@
       <c r="E3" s="52"/>
       <c r="F3" s="52"/>
       <c r="G3" s="53"/>
-      <c r="H3" s="62" t="s">
+      <c r="H3" s="54" t="s">
         <v>199</v>
       </c>
       <c r="I3" s="52"/>
       <c r="J3" s="52"/>
       <c r="K3" s="52"/>
       <c r="L3" s="53"/>
-      <c r="M3" s="57" t="s">
+      <c r="M3" s="58" t="s">
         <v>186</v>
       </c>
       <c r="N3" s="52"/>
       <c r="O3" s="52"/>
       <c r="P3" s="52"/>
       <c r="Q3" s="53"/>
-      <c r="R3" s="60" t="s">
+      <c r="R3" s="59" t="s">
         <v>202</v>
       </c>
       <c r="S3" s="52"/>
@@ -2932,34 +2940,36 @@
       <c r="E4" s="52"/>
       <c r="F4" s="52"/>
       <c r="G4" s="53"/>
-      <c r="H4" s="61" t="s">
-        <v>203</v>
+      <c r="H4" s="65" t="s">
+        <v>210</v>
       </c>
       <c r="I4" s="52"/>
       <c r="J4" s="52"/>
       <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="52"/>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="52"/>
-      <c r="R4" s="52"/>
-      <c r="S4" s="52"/>
-      <c r="T4" s="52"/>
-      <c r="U4" s="52"/>
-      <c r="V4" s="52"/>
-      <c r="W4" s="52"/>
-      <c r="X4" s="52"/>
-      <c r="Y4" s="52"/>
-      <c r="Z4" s="52"/>
-      <c r="AA4" s="52"/>
-      <c r="AB4" s="52"/>
-      <c r="AC4" s="52"/>
-      <c r="AD4" s="52"/>
-      <c r="AE4" s="52"/>
-      <c r="AF4" s="52"/>
-      <c r="AG4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="55" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
+      <c r="V4" s="56"/>
+      <c r="W4" s="56"/>
+      <c r="X4" s="56"/>
+      <c r="Y4" s="56"/>
+      <c r="Z4" s="56"/>
+      <c r="AA4" s="56"/>
+      <c r="AB4" s="56"/>
+      <c r="AC4" s="56"/>
+      <c r="AD4" s="56"/>
+      <c r="AE4" s="56"/>
+      <c r="AF4" s="56"/>
+      <c r="AG4" s="57"/>
     </row>
     <row r="5" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
@@ -2973,21 +2983,21 @@
       <c r="E5" s="52"/>
       <c r="F5" s="52"/>
       <c r="G5" s="53"/>
-      <c r="H5" s="62" t="s">
+      <c r="H5" s="54" t="s">
         <v>204</v>
       </c>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="52"/>
       <c r="L5" s="53"/>
-      <c r="M5" s="57" t="s">
+      <c r="M5" s="58" t="s">
         <v>205</v>
       </c>
       <c r="N5" s="52"/>
       <c r="O5" s="52"/>
       <c r="P5" s="52"/>
       <c r="Q5" s="53"/>
-      <c r="R5" s="60" t="s">
+      <c r="R5" s="59" t="s">
         <v>206</v>
       </c>
       <c r="S5" s="52"/>
@@ -3018,58 +3028,60 @@
       <c r="E6" s="52"/>
       <c r="F6" s="52"/>
       <c r="G6" s="53"/>
-      <c r="H6" s="62" t="s">
+      <c r="H6" s="54" t="s">
         <v>208</v>
       </c>
       <c r="I6" s="52"/>
       <c r="J6" s="52"/>
       <c r="K6" s="52"/>
       <c r="L6" s="53"/>
-      <c r="M6" s="65" t="s">
+      <c r="M6" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="N6" s="63"/>
-      <c r="O6" s="63"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="63"/>
-      <c r="S6" s="63"/>
-      <c r="T6" s="63"/>
-      <c r="U6" s="63"/>
-      <c r="V6" s="63"/>
-      <c r="W6" s="63"/>
-      <c r="X6" s="63"/>
-      <c r="Y6" s="63"/>
-      <c r="Z6" s="63"/>
-      <c r="AA6" s="63"/>
-      <c r="AB6" s="63"/>
-      <c r="AC6" s="63"/>
-      <c r="AD6" s="63"/>
-      <c r="AE6" s="63"/>
-      <c r="AF6" s="63"/>
-      <c r="AG6" s="64"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="56"/>
+      <c r="R6" s="56"/>
+      <c r="S6" s="56"/>
+      <c r="T6" s="56"/>
+      <c r="U6" s="56"/>
+      <c r="V6" s="56"/>
+      <c r="W6" s="56"/>
+      <c r="X6" s="56"/>
+      <c r="Y6" s="56"/>
+      <c r="Z6" s="56"/>
+      <c r="AA6" s="56"/>
+      <c r="AB6" s="56"/>
+      <c r="AC6" s="56"/>
+      <c r="AD6" s="56"/>
+      <c r="AE6" s="56"/>
+      <c r="AF6" s="56"/>
+      <c r="AG6" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="W2:AG2"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="H6:L6"/>
     <mergeCell ref="M6:AG6"/>
     <mergeCell ref="M3:Q3"/>
     <mergeCell ref="R3:AG3"/>
     <mergeCell ref="B4:G4"/>
-    <mergeCell ref="H4:AG4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="H5:L5"/>
     <mergeCell ref="M5:Q5"/>
     <mergeCell ref="R5:AG5"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="H3:L3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="W2:AG2"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="M4:AG4"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated simulator and assembler to use print instructions
</commit_message>
<xml_diff>
--- a/2 - DLX Compiler/Instruction_Set.xlsx
+++ b/2 - DLX Compiler/Instruction_Set.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matthew Crump\Documents\reconfigurable-computing\2 - DLX Compiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF87D21-4CE7-4F45-A2EA-49A556AFEBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBDF4D8-C8B4-4551-B651-AD7AE3252937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="222">
   <si>
     <t>Instruction</t>
   </si>
@@ -654,13 +654,46 @@
   </si>
   <si>
     <t>R31</t>
+  </si>
+  <si>
+    <t>PCH</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>PDU</t>
+  </si>
+  <si>
+    <t>0x31</t>
+  </si>
+  <si>
+    <t>0x32</t>
+  </si>
+  <si>
+    <t>0x33</t>
+  </si>
+  <si>
+    <t>IO</t>
+  </si>
+  <si>
+    <t>Print(rd)</t>
+  </si>
+  <si>
+    <t>Print character</t>
+  </si>
+  <si>
+    <t>Print signed integer</t>
+  </si>
+  <si>
+    <t>Print unsigned integer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -691,8 +724,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -757,6 +795,36 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF3F3F3"/>
         <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCAEBEE"/>
+        <bgColor rgb="FFE8F0FE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCAEBEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCAEBEE"/>
+        <bgColor rgb="FFE0F7FA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5E1CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5E1CC"/>
+        <bgColor rgb="FFE8E7FC"/>
       </patternFill>
     </fill>
   </fills>
@@ -915,7 +983,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1006,6 +1074,9 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1014,10 +1085,35 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1386,6 +1482,12 @@
       <tableStyleElement type="secondRowStripe" dxfId="13"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFC5E1CC"/>
+      <color rgb="FFCAEBEE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1450,7 +1552,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_5" displayName="Table_5" ref="B45:F50" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_5" displayName="Table_5" ref="B45:F53" headerRowCount="0">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Column1" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Column2"/>
@@ -1689,10 +1791,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2644,7 +2746,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>185</v>
       </c>
@@ -2664,7 +2766,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
         <v>190</v>
       </c>
@@ -2684,7 +2786,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>194</v>
       </c>
@@ -2702,6 +2804,66 @@
       </c>
       <c r="F50" s="30" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="78" t="s">
+        <v>211</v>
+      </c>
+      <c r="B51" s="77" t="s">
+        <v>199</v>
+      </c>
+      <c r="C51" s="76" t="s">
+        <v>219</v>
+      </c>
+      <c r="D51" s="76" t="s">
+        <v>218</v>
+      </c>
+      <c r="E51" s="75" t="s">
+        <v>214</v>
+      </c>
+      <c r="F51" s="75" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="50" t="s">
+        <v>212</v>
+      </c>
+      <c r="B52" s="73" t="s">
+        <v>199</v>
+      </c>
+      <c r="C52" s="74" t="s">
+        <v>220</v>
+      </c>
+      <c r="D52" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="E52" s="72" t="s">
+        <v>215</v>
+      </c>
+      <c r="F52" s="72" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="78" t="s">
+        <v>213</v>
+      </c>
+      <c r="B53" s="77" t="s">
+        <v>199</v>
+      </c>
+      <c r="C53" s="79" t="s">
+        <v>221</v>
+      </c>
+      <c r="D53" s="79" t="s">
+        <v>218</v>
+      </c>
+      <c r="E53" s="80" t="s">
+        <v>216</v>
+      </c>
+      <c r="F53" s="81" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2724,10 +2886,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AG6"/>
+  <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2848,13 +3010,13 @@
       <c r="E2" s="52"/>
       <c r="F2" s="52"/>
       <c r="G2" s="53"/>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="61" t="s">
         <v>199</v>
       </c>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="63"/>
       <c r="M2" s="58" t="s">
         <v>186</v>
       </c>
@@ -2862,26 +3024,26 @@
       <c r="O2" s="52"/>
       <c r="P2" s="52"/>
       <c r="Q2" s="53"/>
-      <c r="R2" s="63" t="s">
+      <c r="R2" s="64" t="s">
         <v>200</v>
       </c>
       <c r="S2" s="52"/>
       <c r="T2" s="52"/>
       <c r="U2" s="52"/>
       <c r="V2" s="53"/>
-      <c r="W2" s="64" t="s">
+      <c r="W2" s="69" t="s">
         <v>201</v>
       </c>
-      <c r="X2" s="52"/>
-      <c r="Y2" s="52"/>
-      <c r="Z2" s="52"/>
-      <c r="AA2" s="52"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="52"/>
-      <c r="AD2" s="52"/>
-      <c r="AE2" s="52"/>
-      <c r="AF2" s="52"/>
-      <c r="AG2" s="53"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="70"/>
+      <c r="AA2" s="70"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="70"/>
+      <c r="AF2" s="70"/>
+      <c r="AG2" s="71"/>
     </row>
     <row r="3" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -2940,7 +3102,7 @@
       <c r="E4" s="52"/>
       <c r="F4" s="52"/>
       <c r="G4" s="53"/>
-      <c r="H4" s="65" t="s">
+      <c r="H4" s="60" t="s">
         <v>210</v>
       </c>
       <c r="I4" s="52"/>
@@ -3059,8 +3221,54 @@
       <c r="AF6" s="56"/>
       <c r="AG6" s="57"/>
     </row>
+    <row r="7" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="65" t="s">
+        <v>217</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="60" t="s">
+        <v>199</v>
+      </c>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="66" t="s">
+        <v>201</v>
+      </c>
+      <c r="N7" s="67"/>
+      <c r="O7" s="67"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
+      <c r="S7" s="67"/>
+      <c r="T7" s="67"/>
+      <c r="U7" s="67"/>
+      <c r="V7" s="67"/>
+      <c r="W7" s="67"/>
+      <c r="X7" s="67"/>
+      <c r="Y7" s="67"/>
+      <c r="Z7" s="67"/>
+      <c r="AA7" s="67"/>
+      <c r="AB7" s="67"/>
+      <c r="AC7" s="67"/>
+      <c r="AD7" s="67"/>
+      <c r="AE7" s="67"/>
+      <c r="AF7" s="67"/>
+      <c r="AG7" s="68"/>
+    </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="22">
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="M7:AG7"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="M2:Q2"/>

</xml_diff>

<commit_message>
Fixed last print issues.
</commit_message>
<xml_diff>
--- a/2 - DLX Compiler/Instruction_Set.xlsx
+++ b/2 - DLX Compiler/Instruction_Set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matthew Crump\Documents\reconfigurable-computing\2 - DLX Compiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBDF4D8-C8B4-4551-B651-AD7AE3252937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A9C006-CC9B-42F5-BF98-E891C773A9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5445" yWindow="3270" windowWidth="16695" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="222">
   <si>
     <t>Instruction</t>
   </si>
@@ -693,7 +693,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -729,8 +729,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -795,12 +801,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF3F3F3"/>
         <bgColor rgb="FFF3F3F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCAEBEE"/>
-        <bgColor rgb="FFE8F0FE"/>
       </patternFill>
     </fill>
     <fill>
@@ -1055,11 +1055,51 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1068,52 +1108,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1793,7 +1797,7 @@
   </sheetPr>
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
@@ -2807,22 +2811,22 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="78" t="s">
+      <c r="A51" s="58" t="s">
         <v>211</v>
       </c>
-      <c r="B51" s="77" t="s">
+      <c r="B51" s="57" t="s">
         <v>199</v>
       </c>
-      <c r="C51" s="76" t="s">
+      <c r="C51" s="56" t="s">
         <v>219</v>
       </c>
-      <c r="D51" s="76" t="s">
+      <c r="D51" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="E51" s="75" t="s">
+      <c r="E51" s="55" t="s">
         <v>214</v>
       </c>
-      <c r="F51" s="75" t="s">
+      <c r="F51" s="55" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2830,39 +2834,39 @@
       <c r="A52" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="B52" s="73" t="s">
+      <c r="B52" s="53" t="s">
         <v>199</v>
       </c>
-      <c r="C52" s="74" t="s">
+      <c r="C52" s="54" t="s">
         <v>220</v>
       </c>
-      <c r="D52" s="74" t="s">
+      <c r="D52" s="54" t="s">
         <v>218</v>
       </c>
-      <c r="E52" s="72" t="s">
+      <c r="E52" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="F52" s="72" t="s">
+      <c r="F52" s="52" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="78" t="s">
+      <c r="A53" s="58" t="s">
         <v>213</v>
       </c>
-      <c r="B53" s="77" t="s">
+      <c r="B53" s="57" t="s">
         <v>199</v>
       </c>
-      <c r="C53" s="79" t="s">
+      <c r="C53" s="59" t="s">
         <v>221</v>
       </c>
-      <c r="D53" s="79" t="s">
+      <c r="D53" s="59" t="s">
         <v>218</v>
       </c>
-      <c r="E53" s="80" t="s">
+      <c r="E53" s="60" t="s">
         <v>216</v>
       </c>
-      <c r="F53" s="81" t="s">
+      <c r="F53" s="61" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2888,8 +2892,8 @@
   </sheetPr>
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P13:P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3002,273 +3006,282 @@
       <c r="A2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="62" t="s">
         <v>198</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="61" t="s">
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="66" t="s">
         <v>199</v>
       </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="58" t="s">
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69" t="s">
         <v>186</v>
       </c>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="64" t="s">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="70" t="s">
         <v>200</v>
       </c>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="69" t="s">
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="64"/>
+      <c r="W2" s="71" t="s">
         <v>201</v>
       </c>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="70"/>
-      <c r="AA2" s="70"/>
-      <c r="AB2" s="70"/>
-      <c r="AC2" s="70"/>
-      <c r="AD2" s="70"/>
-      <c r="AE2" s="70"/>
-      <c r="AF2" s="70"/>
-      <c r="AG2" s="71"/>
+      <c r="X2" s="72"/>
+      <c r="Y2" s="72"/>
+      <c r="Z2" s="72"/>
+      <c r="AA2" s="72"/>
+      <c r="AB2" s="72"/>
+      <c r="AC2" s="72"/>
+      <c r="AD2" s="72"/>
+      <c r="AE2" s="72"/>
+      <c r="AF2" s="72"/>
+      <c r="AG2" s="73"/>
     </row>
     <row r="3" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="62" t="s">
         <v>198</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="54" t="s">
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="74" t="s">
         <v>199</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="58" t="s">
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="69" t="s">
         <v>186</v>
       </c>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="59" t="s">
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="78" t="s">
         <v>202</v>
       </c>
-      <c r="S3" s="52"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52"/>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52"/>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="52"/>
-      <c r="Z3" s="52"/>
-      <c r="AA3" s="52"/>
-      <c r="AB3" s="52"/>
-      <c r="AC3" s="52"/>
-      <c r="AD3" s="52"/>
-      <c r="AE3" s="52"/>
-      <c r="AF3" s="52"/>
-      <c r="AG3" s="53"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
+      <c r="V3" s="63"/>
+      <c r="W3" s="63"/>
+      <c r="X3" s="63"/>
+      <c r="Y3" s="63"/>
+      <c r="Z3" s="63"/>
+      <c r="AA3" s="63"/>
+      <c r="AB3" s="63"/>
+      <c r="AC3" s="63"/>
+      <c r="AD3" s="63"/>
+      <c r="AE3" s="63"/>
+      <c r="AF3" s="63"/>
+      <c r="AG3" s="64"/>
     </row>
     <row r="4" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="62" t="s">
         <v>198</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="60" t="s">
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="65" t="s">
         <v>210</v>
       </c>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="55" t="s">
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="75" t="s">
         <v>203</v>
       </c>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="56"/>
-      <c r="T4" s="56"/>
-      <c r="U4" s="56"/>
-      <c r="V4" s="56"/>
-      <c r="W4" s="56"/>
-      <c r="X4" s="56"/>
-      <c r="Y4" s="56"/>
-      <c r="Z4" s="56"/>
-      <c r="AA4" s="56"/>
-      <c r="AB4" s="56"/>
-      <c r="AC4" s="56"/>
-      <c r="AD4" s="56"/>
-      <c r="AE4" s="56"/>
-      <c r="AF4" s="56"/>
-      <c r="AG4" s="57"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="76"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="76"/>
+      <c r="AC4" s="76"/>
+      <c r="AD4" s="76"/>
+      <c r="AE4" s="76"/>
+      <c r="AF4" s="76"/>
+      <c r="AG4" s="77"/>
     </row>
     <row r="5" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="62" t="s">
         <v>198</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="54" t="s">
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="74" t="s">
         <v>204</v>
       </c>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="58" t="s">
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="69" t="s">
         <v>205</v>
       </c>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="59" t="s">
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="64"/>
+      <c r="R5" s="78" t="s">
         <v>206</v>
       </c>
-      <c r="S5" s="52"/>
-      <c r="T5" s="52"/>
-      <c r="U5" s="52"/>
-      <c r="V5" s="52"/>
-      <c r="W5" s="52"/>
-      <c r="X5" s="52"/>
-      <c r="Y5" s="52"/>
-      <c r="Z5" s="52"/>
-      <c r="AA5" s="52"/>
-      <c r="AB5" s="52"/>
-      <c r="AC5" s="52"/>
-      <c r="AD5" s="52"/>
-      <c r="AE5" s="52"/>
-      <c r="AF5" s="52"/>
-      <c r="AG5" s="53"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
+      <c r="V5" s="63"/>
+      <c r="W5" s="63"/>
+      <c r="X5" s="63"/>
+      <c r="Y5" s="63"/>
+      <c r="Z5" s="63"/>
+      <c r="AA5" s="63"/>
+      <c r="AB5" s="63"/>
+      <c r="AC5" s="63"/>
+      <c r="AD5" s="63"/>
+      <c r="AE5" s="63"/>
+      <c r="AF5" s="63"/>
+      <c r="AG5" s="64"/>
     </row>
     <row r="6" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="62" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="54" t="s">
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="74" t="s">
         <v>208</v>
       </c>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="55" t="s">
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="75" t="s">
         <v>209</v>
       </c>
-      <c r="N6" s="56"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="56"/>
-      <c r="S6" s="56"/>
-      <c r="T6" s="56"/>
-      <c r="U6" s="56"/>
-      <c r="V6" s="56"/>
-      <c r="W6" s="56"/>
-      <c r="X6" s="56"/>
-      <c r="Y6" s="56"/>
-      <c r="Z6" s="56"/>
-      <c r="AA6" s="56"/>
-      <c r="AB6" s="56"/>
-      <c r="AC6" s="56"/>
-      <c r="AD6" s="56"/>
-      <c r="AE6" s="56"/>
-      <c r="AF6" s="56"/>
-      <c r="AG6" s="57"/>
+      <c r="N6" s="76"/>
+      <c r="O6" s="76"/>
+      <c r="P6" s="76"/>
+      <c r="Q6" s="76"/>
+      <c r="R6" s="76"/>
+      <c r="S6" s="76"/>
+      <c r="T6" s="76"/>
+      <c r="U6" s="76"/>
+      <c r="V6" s="76"/>
+      <c r="W6" s="76"/>
+      <c r="X6" s="76"/>
+      <c r="Y6" s="76"/>
+      <c r="Z6" s="76"/>
+      <c r="AA6" s="76"/>
+      <c r="AB6" s="76"/>
+      <c r="AC6" s="76"/>
+      <c r="AD6" s="76"/>
+      <c r="AE6" s="76"/>
+      <c r="AF6" s="76"/>
+      <c r="AG6" s="77"/>
     </row>
     <row r="7" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="51" t="s">
         <v>217</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="62" t="s">
         <v>198</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="60" t="s">
-        <v>199</v>
-      </c>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="66" t="s">
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="79" t="s">
         <v>201</v>
       </c>
-      <c r="N7" s="67"/>
-      <c r="O7" s="67"/>
-      <c r="P7" s="67"/>
-      <c r="Q7" s="67"/>
-      <c r="R7" s="67"/>
-      <c r="S7" s="67"/>
-      <c r="T7" s="67"/>
-      <c r="U7" s="67"/>
-      <c r="V7" s="67"/>
-      <c r="W7" s="67"/>
-      <c r="X7" s="67"/>
-      <c r="Y7" s="67"/>
-      <c r="Z7" s="67"/>
-      <c r="AA7" s="67"/>
-      <c r="AB7" s="67"/>
-      <c r="AC7" s="67"/>
-      <c r="AD7" s="67"/>
-      <c r="AE7" s="67"/>
-      <c r="AF7" s="67"/>
-      <c r="AG7" s="68"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="69" t="s">
+        <v>186</v>
+      </c>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="64"/>
+      <c r="R7" s="79" t="s">
+        <v>201</v>
+      </c>
+      <c r="S7" s="80"/>
+      <c r="T7" s="80"/>
+      <c r="U7" s="80"/>
+      <c r="V7" s="80"/>
+      <c r="W7" s="80"/>
+      <c r="X7" s="80"/>
+      <c r="Y7" s="80"/>
+      <c r="Z7" s="80"/>
+      <c r="AA7" s="80"/>
+      <c r="AB7" s="80"/>
+      <c r="AC7" s="80"/>
+      <c r="AD7" s="80"/>
+      <c r="AE7" s="80"/>
+      <c r="AF7" s="80"/>
+      <c r="AG7" s="81"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="23">
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="R7:AG7"/>
+    <mergeCell ref="M5:Q5"/>
+    <mergeCell ref="R5:AG5"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="M4:AG4"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="M7:AG7"/>
+    <mergeCell ref="M7:Q7"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="M2:Q2"/>
@@ -3282,12 +3295,6 @@
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="H5:L5"/>
-    <mergeCell ref="M5:Q5"/>
-    <mergeCell ref="R5:AG5"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="M4:AG4"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated compiler and example to include scan instructions
</commit_message>
<xml_diff>
--- a/2 - DLX Compiler/Instruction_Set.xlsx
+++ b/2 - DLX Compiler/Instruction_Set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matthew Crump\Documents\reconfigurable-computing\2 - DLX Compiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A9C006-CC9B-42F5-BF98-E891C773A9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6611893C-3919-4EA8-BD47-87F1E919941A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="3270" windowWidth="16695" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="229">
   <si>
     <t>Instruction</t>
   </si>
@@ -687,6 +687,27 @@
   </si>
   <si>
     <t>Print unsigned integer</t>
+  </si>
+  <si>
+    <t>GD</t>
+  </si>
+  <si>
+    <t>GDU</t>
+  </si>
+  <si>
+    <t>Get signed decimal</t>
+  </si>
+  <si>
+    <t>Get unsigned decimal</t>
+  </si>
+  <si>
+    <t>rd = Get()</t>
+  </si>
+  <si>
+    <t>0x34</t>
+  </si>
+  <si>
+    <t>0x35</t>
   </si>
 </sst>
 </file>
@@ -1076,41 +1097,6 @@
     <xf numFmtId="0" fontId="6" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1120,6 +1106,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1795,10 +1816,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2867,6 +2888,46 @@
         <v>216</v>
       </c>
       <c r="F53" s="61" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="B54" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="C54" s="54" t="s">
+        <v>224</v>
+      </c>
+      <c r="D54" s="54" t="s">
+        <v>226</v>
+      </c>
+      <c r="E54" s="52" t="s">
+        <v>227</v>
+      </c>
+      <c r="F54" s="52" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="58" t="s">
+        <v>223</v>
+      </c>
+      <c r="B55" s="57" t="s">
+        <v>199</v>
+      </c>
+      <c r="C55" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="D55" s="59" t="s">
+        <v>226</v>
+      </c>
+      <c r="E55" s="60" t="s">
+        <v>228</v>
+      </c>
+      <c r="F55" s="61" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2892,7 +2953,7 @@
   </sheetPr>
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P14" sqref="P13:P14"/>
     </sheetView>
   </sheetViews>
@@ -3006,272 +3067,279 @@
       <c r="A2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="69" t="s">
         <v>198</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="66" t="s">
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="75" t="s">
         <v>199</v>
       </c>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="69" t="s">
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="65" t="s">
         <v>186</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="70" t="s">
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="78" t="s">
         <v>200</v>
       </c>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="64"/>
-      <c r="W2" s="71" t="s">
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="67"/>
+      <c r="W2" s="79" t="s">
         <v>201</v>
       </c>
-      <c r="X2" s="72"/>
-      <c r="Y2" s="72"/>
-      <c r="Z2" s="72"/>
-      <c r="AA2" s="72"/>
-      <c r="AB2" s="72"/>
-      <c r="AC2" s="72"/>
-      <c r="AD2" s="72"/>
-      <c r="AE2" s="72"/>
-      <c r="AF2" s="72"/>
-      <c r="AG2" s="73"/>
+      <c r="X2" s="80"/>
+      <c r="Y2" s="80"/>
+      <c r="Z2" s="80"/>
+      <c r="AA2" s="80"/>
+      <c r="AB2" s="80"/>
+      <c r="AC2" s="80"/>
+      <c r="AD2" s="80"/>
+      <c r="AE2" s="80"/>
+      <c r="AF2" s="80"/>
+      <c r="AG2" s="81"/>
     </row>
     <row r="3" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="69" t="s">
         <v>198</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="74" t="s">
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="70" t="s">
         <v>199</v>
       </c>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="69" t="s">
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="65" t="s">
         <v>186</v>
       </c>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="78" t="s">
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="66"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="68" t="s">
         <v>202</v>
       </c>
-      <c r="S3" s="63"/>
-      <c r="T3" s="63"/>
-      <c r="U3" s="63"/>
-      <c r="V3" s="63"/>
-      <c r="W3" s="63"/>
-      <c r="X3" s="63"/>
-      <c r="Y3" s="63"/>
-      <c r="Z3" s="63"/>
-      <c r="AA3" s="63"/>
-      <c r="AB3" s="63"/>
-      <c r="AC3" s="63"/>
-      <c r="AD3" s="63"/>
-      <c r="AE3" s="63"/>
-      <c r="AF3" s="63"/>
-      <c r="AG3" s="64"/>
+      <c r="S3" s="66"/>
+      <c r="T3" s="66"/>
+      <c r="U3" s="66"/>
+      <c r="V3" s="66"/>
+      <c r="W3" s="66"/>
+      <c r="X3" s="66"/>
+      <c r="Y3" s="66"/>
+      <c r="Z3" s="66"/>
+      <c r="AA3" s="66"/>
+      <c r="AB3" s="66"/>
+      <c r="AC3" s="66"/>
+      <c r="AD3" s="66"/>
+      <c r="AE3" s="66"/>
+      <c r="AF3" s="66"/>
+      <c r="AG3" s="67"/>
     </row>
     <row r="4" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="69" t="s">
         <v>198</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="65" t="s">
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="71" t="s">
         <v>210</v>
       </c>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="75" t="s">
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="72" t="s">
         <v>203</v>
       </c>
-      <c r="N4" s="76"/>
-      <c r="O4" s="76"/>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="76"/>
-      <c r="R4" s="76"/>
-      <c r="S4" s="76"/>
-      <c r="T4" s="76"/>
-      <c r="U4" s="76"/>
-      <c r="V4" s="76"/>
-      <c r="W4" s="76"/>
-      <c r="X4" s="76"/>
-      <c r="Y4" s="76"/>
-      <c r="Z4" s="76"/>
-      <c r="AA4" s="76"/>
-      <c r="AB4" s="76"/>
-      <c r="AC4" s="76"/>
-      <c r="AD4" s="76"/>
-      <c r="AE4" s="76"/>
-      <c r="AF4" s="76"/>
-      <c r="AG4" s="77"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73"/>
+      <c r="R4" s="73"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="73"/>
+      <c r="V4" s="73"/>
+      <c r="W4" s="73"/>
+      <c r="X4" s="73"/>
+      <c r="Y4" s="73"/>
+      <c r="Z4" s="73"/>
+      <c r="AA4" s="73"/>
+      <c r="AB4" s="73"/>
+      <c r="AC4" s="73"/>
+      <c r="AD4" s="73"/>
+      <c r="AE4" s="73"/>
+      <c r="AF4" s="73"/>
+      <c r="AG4" s="74"/>
     </row>
     <row r="5" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="69" t="s">
         <v>198</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="74" t="s">
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="70" t="s">
         <v>204</v>
       </c>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="69" t="s">
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="65" t="s">
         <v>205</v>
       </c>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="63"/>
-      <c r="Q5" s="64"/>
-      <c r="R5" s="78" t="s">
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="68" t="s">
         <v>206</v>
       </c>
-      <c r="S5" s="63"/>
-      <c r="T5" s="63"/>
-      <c r="U5" s="63"/>
-      <c r="V5" s="63"/>
-      <c r="W5" s="63"/>
-      <c r="X5" s="63"/>
-      <c r="Y5" s="63"/>
-      <c r="Z5" s="63"/>
-      <c r="AA5" s="63"/>
-      <c r="AB5" s="63"/>
-      <c r="AC5" s="63"/>
-      <c r="AD5" s="63"/>
-      <c r="AE5" s="63"/>
-      <c r="AF5" s="63"/>
-      <c r="AG5" s="64"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="66"/>
+      <c r="W5" s="66"/>
+      <c r="X5" s="66"/>
+      <c r="Y5" s="66"/>
+      <c r="Z5" s="66"/>
+      <c r="AA5" s="66"/>
+      <c r="AB5" s="66"/>
+      <c r="AC5" s="66"/>
+      <c r="AD5" s="66"/>
+      <c r="AE5" s="66"/>
+      <c r="AF5" s="66"/>
+      <c r="AG5" s="67"/>
     </row>
     <row r="6" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="69" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="74" t="s">
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="70" t="s">
         <v>208</v>
       </c>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="75" t="s">
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="72" t="s">
         <v>209</v>
       </c>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="76"/>
-      <c r="R6" s="76"/>
-      <c r="S6" s="76"/>
-      <c r="T6" s="76"/>
-      <c r="U6" s="76"/>
-      <c r="V6" s="76"/>
-      <c r="W6" s="76"/>
-      <c r="X6" s="76"/>
-      <c r="Y6" s="76"/>
-      <c r="Z6" s="76"/>
-      <c r="AA6" s="76"/>
-      <c r="AB6" s="76"/>
-      <c r="AC6" s="76"/>
-      <c r="AD6" s="76"/>
-      <c r="AE6" s="76"/>
-      <c r="AF6" s="76"/>
-      <c r="AG6" s="77"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="73"/>
+      <c r="S6" s="73"/>
+      <c r="T6" s="73"/>
+      <c r="U6" s="73"/>
+      <c r="V6" s="73"/>
+      <c r="W6" s="73"/>
+      <c r="X6" s="73"/>
+      <c r="Y6" s="73"/>
+      <c r="Z6" s="73"/>
+      <c r="AA6" s="73"/>
+      <c r="AB6" s="73"/>
+      <c r="AC6" s="73"/>
+      <c r="AD6" s="73"/>
+      <c r="AE6" s="73"/>
+      <c r="AF6" s="73"/>
+      <c r="AG6" s="74"/>
     </row>
     <row r="7" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="51" t="s">
         <v>217</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="69" t="s">
         <v>198</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="79" t="s">
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="69" t="s">
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="65" t="s">
         <v>186</v>
       </c>
-      <c r="N7" s="63"/>
-      <c r="O7" s="63"/>
-      <c r="P7" s="63"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="79" t="s">
+      <c r="N7" s="66"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="S7" s="80"/>
-      <c r="T7" s="80"/>
-      <c r="U7" s="80"/>
-      <c r="V7" s="80"/>
-      <c r="W7" s="80"/>
-      <c r="X7" s="80"/>
-      <c r="Y7" s="80"/>
-      <c r="Z7" s="80"/>
-      <c r="AA7" s="80"/>
-      <c r="AB7" s="80"/>
-      <c r="AC7" s="80"/>
-      <c r="AD7" s="80"/>
-      <c r="AE7" s="80"/>
-      <c r="AF7" s="80"/>
-      <c r="AG7" s="81"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="63"/>
+      <c r="W7" s="63"/>
+      <c r="X7" s="63"/>
+      <c r="Y7" s="63"/>
+      <c r="Z7" s="63"/>
+      <c r="AA7" s="63"/>
+      <c r="AB7" s="63"/>
+      <c r="AC7" s="63"/>
+      <c r="AD7" s="63"/>
+      <c r="AE7" s="63"/>
+      <c r="AF7" s="63"/>
+      <c r="AG7" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="W2:AG2"/>
     <mergeCell ref="H7:L7"/>
     <mergeCell ref="R7:AG7"/>
     <mergeCell ref="M5:Q5"/>
@@ -3282,19 +3350,12 @@
     <mergeCell ref="M4:AG4"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="M7:Q7"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="W2:AG2"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="H6:L6"/>
     <mergeCell ref="M6:AG6"/>
     <mergeCell ref="M3:Q3"/>
     <mergeCell ref="R3:AG3"/>
     <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="H5:L5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>